<commit_message>
Added output data table
</commit_message>
<xml_diff>
--- a/Employees Data.xlsx
+++ b/Employees Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20400"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/ashritha_bhaskar_uipath_com/Documents/Documents/UiPath/Filter Employees Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charlie\OneDrive\Documents\UiPath Advance\Filter Employee Data Using Select Method\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{5B71F57A-E9A1-43A3-88E3-653A93D8EC50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ED863764-70B7-47A2-BB7D-0283AC824E81}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC7E8BBE-62EF-4B40-A9DC-E70090E2E732}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -621,21 +621,21 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.33203125" customWidth="1"/>
+    <col min="1" max="1" width="30.28515625" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="21.109375" customWidth="1"/>
-    <col min="4" max="4" width="16.44140625" customWidth="1"/>
-    <col min="5" max="5" width="18.21875" customWidth="1"/>
-    <col min="6" max="6" width="33.44140625" customWidth="1"/>
-    <col min="7" max="7" width="34.6640625" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="33.42578125" customWidth="1"/>
+    <col min="7" max="7" width="34.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -658,7 +658,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
@@ -681,7 +681,7 @@
         <v>40716543298</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>12</v>
       </c>
@@ -704,7 +704,7 @@
         <v>40791345621</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>17</v>
       </c>
@@ -727,7 +727,7 @@
         <v>40735416854</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>22</v>
       </c>
@@ -750,7 +750,7 @@
         <v>40733652145</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>46</v>
       </c>
@@ -773,7 +773,7 @@
         <v>40799885412</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>29</v>
       </c>
@@ -796,7 +796,7 @@
         <v>40733154268</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>12</v>
       </c>
@@ -819,7 +819,7 @@
         <v>40712462257</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>38</v>
       </c>
@@ -842,7 +842,7 @@
         <v>40731254562</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>41</v>
       </c>
@@ -865,7 +865,7 @@
         <v>40741785214</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>46</v>
       </c>

</xml_diff>